<commit_message>
sort excel: table right side can be sort but left side not
</commit_message>
<xml_diff>
--- a/sort12-3-25.xlsx
+++ b/sort12-3-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LEARN MS OFFICE\EXCEL\excel practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4AB9B-8E0E-4B3B-B13C-889DED8A75B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A4BEBA-693B-4351-AEE8-E4FFED2D9634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3DAFC8C4-3BA1-47CA-96F3-A4216C8E4A71}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>salary based sorting by ascending orders</t>
+  </si>
+  <si>
+    <t>try to sort 2 or 3 columns not entire column</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E83DFF-2EBC-47AE-9E6F-2FA1521A96D4}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +484,7 @@
     <col min="3" max="3" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -503,7 +506,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -514,7 +517,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -525,7 +528,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -536,7 +539,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -545,7 +548,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="str" cm="1">
         <f t="array" ref="A10:C13">_xlfn._xlws.SORT(A2:C5,3,1)</f>
         <v>Bob</v>
@@ -568,7 +571,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <v>John</v>
       </c>
@@ -579,7 +582,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <v>Alice</v>
       </c>
@@ -590,7 +593,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <v>Carol</v>
       </c>
@@ -601,9 +604,61 @@
         <v>7000</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="23" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="str" cm="1">
+        <f t="array" ref="A17:B20">_xlfn._xlws.SORT(B2:C5,2,1)</f>
+        <v>Sales</v>
+      </c>
+      <c r="B17">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="B18">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="str">
+        <v>HR</v>
+      </c>
+      <c r="B19">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="str">
+        <v>IT</v>
+      </c>
+      <c r="B20">
+        <v>7000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A7:E7"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>